<commit_message>
Agregada la forma de resolución del ítem 9.
</commit_message>
<xml_diff>
--- a/Documentacion/Planificacion.xlsx
+++ b/Documentacion/Planificacion.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="18735" windowHeight="8640"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="18735" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprints" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Descripcion estado</t>
-  </si>
-  <si>
-    <t>Por comenzar</t>
   </si>
   <si>
     <t>Hay que cambiar los campos
@@ -268,15 +265,22 @@
   <si>
     <t>Ver permisos</t>
   </si>
+  <si>
+    <t>Utilizar el campo grade_export_decimalpoints, agregar opción hasta 10 cuatrimestres y reemplazar la descripción
+Reemplazar "Reiniciar" el curso por "Consolidar Cuatrimestre"
+Cuando se ejecuta, crear o hacer un append a un archivo CSV para las calificaciones de la materia, indicar número de cuatrimestre
+Para mostrar calificaciones de cuatrimestres anteriores, reemplazar la pantalla de Informe General
+                  Acceder al CSV de la materia y listar en función del parámetro de cantidad de cuatrimestres de conservación configurado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,21 +418,24 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:R36" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:R36">
-    <filterColumn colId="0"/>
-    <filterColumn colId="2"/>
     <filterColumn colId="3">
       <filters>
         <filter val="1"/>
@@ -545,6 +552,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -579,6 +587,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,14 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="97.28515625" bestFit="1" customWidth="1"/>
@@ -776,7 +785,7 @@
     <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -832,7 +841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -846,7 +855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -874,7 +883,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" hidden="1">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -902,7 +911,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" hidden="1">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -930,7 +939,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -958,7 +967,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -986,7 +995,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1014,7 +1023,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1042,7 +1051,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" ht="30">
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1059,7 +1068,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:18" hidden="1">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1087,7 +1096,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1115,7 +1124,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1143,7 +1152,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" hidden="1">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1171,7 +1180,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="45" hidden="1">
+    <row r="15" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1199,7 +1208,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1216,7 +1225,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1233,7 +1242,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1261,7 +1270,7 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" hidden="1">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1289,7 +1298,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:18" hidden="1">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1317,7 +1326,7 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" ht="30" hidden="1">
+    <row r="21" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1331,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" hidden="1">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1359,7 +1368,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" ht="30" hidden="1">
+    <row r="23" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1373,7 +1382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1387,7 +1396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1415,7 +1424,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" hidden="1">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1443,7 +1452,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" hidden="1">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1471,7 +1480,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1499,7 +1508,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:18" hidden="1">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30" hidden="1">
+    <row r="30" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1541,7 +1550,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" hidden="1">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1555,7 +1564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1583,7 +1592,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" hidden="1">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1611,7 +1620,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="1:18" hidden="1">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1639,7 +1648,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1667,12 +1676,12 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2">
@@ -1703,19 +1712,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="191.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1723,119 +1732,119 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="255">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
     </row>
@@ -1849,34 +1858,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" thickBot="1">
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1"/>
-    <row r="3" spans="1:2">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Documente eso que habia dicho por mail
</commit_message>
<xml_diff>
--- a/Documentacion/Planificacion.xlsx
+++ b/Documentacion/Planificacion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="18735" windowHeight="8640" activeTab="1"/>
@@ -11,7 +11,10 @@
     <sheet name="DetalleFuncionalidades" sheetId="2" r:id="rId2"/>
     <sheet name="Descripcion" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DetalleFuncionalidades!$A$1:$B$16</definedName>
+  </definedNames>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
@@ -213,15 +216,52 @@
     <t>Administrador -&gt; Administracion del sitio -&gt; Usuarios -&gt; Hojear la lista de usuarios</t>
   </si>
   <si>
+    <t>Idem 8</t>
+  </si>
+  <si>
+    <t>Administración de roles</t>
+  </si>
+  <si>
+    <t>Administracion del sitio -&gt; Cursos -&gt; Agregar/editar cursos
+Cambiar Categoría por Materias
+Sacar boton Agregar una sub-categoría
+Limpiar el menu de creación de cursos</t>
+  </si>
+  <si>
+    <t>Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Usuarios Matriculados -&gt; Matricular Usuario
+Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Asignar roles -&gt; Profesor</t>
+  </si>
+  <si>
+    <t>Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Usuarios Matriculados  -&gt; Metodos de matriculacion -&gt; Agregar auto matriculacion
+En el código de auto matriculación guardar en una tabla los pendientes y que el codigo siguiente lo haga el mediador</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Idem 27</t>
+  </si>
+  <si>
+    <t>Ver permisos</t>
+  </si>
+  <si>
+    <t>Utilizar el campo grade_export_decimalpoints, agregar opción hasta 10 cuatrimestres y reemplazar la descripción
+Reemplazar "Reiniciar" el curso por "Consolidar Cuatrimestre"
+Cuando se ejecuta, crear o hacer un append a un archivo CSV para las calificaciones de la materia, indicar número de cuatrimestre
+Para mostrar calificaciones de cuatrimestres anteriores, reemplazar la pantalla de Informe General
+                  Acceder al CSV de la materia y listar en función del parámetro de cantidad de cuatrimestres de conservación configurado</t>
+  </si>
+  <si>
     <t>Administrador -&gt; Pagina Principal -&gt; Editar Ajustes -&gt; Página Principal -&gt; Cambiar Mostrar lista de cursos por Mostrar lista de noticias
 Lo mismo para frontpageloggedin
-Cambiar lista de item a mostrar a 10</t>
-  </si>
-  <si>
-    <t>Idem 8</t>
-  </si>
-  <si>
-    <t>Administración de roles</t>
+Cambiar lista de item a mostrar a 10
+Administrador -&gt; Pagina Principal -&gt; Informes -&gt; Novedades del sitio -&gt; Ajustes -&gt; Editar Ajustes -&gt; Cambiar:
+Area General
+       Nombre del foro: Cartelera General
+       Introduccion: Noticias
+       Modalidad de suscripción : Suscripcion deshabilitada
+       Tamaño máximo del archivo adjunto: Nose permite subir archivos
+       Número máximo de archivos adjuntos : 0</t>
   </si>
   <si>
     <t xml:space="preserve">Administracio del sitio -&gt; Usuario -&gt; Permisos -&gt; Politicas del usuario
@@ -240,50 +280,35 @@
       Cambiar nombre de rol
 Estudiante
       Cambiar nombre a aprendiz
+Administrador -&gt; Administración del sitio -&gt; Características Avanzadas -&gt; Cambiar:
+      Deshabilitar Comentarios y Funcionalidad de Marcas
+      Visibilidad del blog: Deshabilitar por completo el sistema blog
       </t>
-  </si>
-  <si>
-    <t>Administracion del sitio -&gt; Cursos -&gt; Agregar/editar cursos
-Cambiar Categoría por Materias
-Sacar boton Agregar una sub-categoría
-Limpiar el menu de creación de cursos</t>
-  </si>
-  <si>
-    <t>Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Usuarios Matriculados -&gt; Matricular Usuario
-Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Asignar roles -&gt; Profesor</t>
-  </si>
-  <si>
-    <t>Administrador -&gt; Administracion del curso -&gt; Usuarios -&gt; Usuarios Matriculados  -&gt; Metodos de matriculacion -&gt; Agregar auto matriculacion
-En el código de auto matriculación guardar en una tabla los pendientes y que el codigo siguiente lo haga el mediador</t>
-  </si>
-  <si>
-    <t>Finalizado</t>
-  </si>
-  <si>
-    <t>Idem 27</t>
-  </si>
-  <si>
-    <t>Ver permisos</t>
-  </si>
-  <si>
-    <t>Utilizar el campo grade_export_decimalpoints, agregar opción hasta 10 cuatrimestres y reemplazar la descripción
-Reemplazar "Reiniciar" el curso por "Consolidar Cuatrimestre"
-Cuando se ejecuta, crear o hacer un append a un archivo CSV para las calificaciones de la materia, indicar número de cuatrimestre
-Para mostrar calificaciones de cuatrimestres anteriores, reemplazar la pantalla de Informe General
-                  Acceder al CSV de la materia y listar en función del parámetro de cantidad de cuatrimestres de conservación configurado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,13 +325,6 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,6 +354,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
@@ -344,18 +367,28 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="63"/>
+      </left>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top style="thin">
+        <color indexed="63"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -385,11 +418,11 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -401,40 +434,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Buena" xfId="3" builtinId="26"/>
-    <cellStyle name="Encabezado 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Heading 4" xfId="3" builtinId="19"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Salida" xfId="5" builtinId="21"/>
-    <cellStyle name="Título 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Output" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:R36" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:R36" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:R36">
     <filterColumn colId="3">
       <filters>
@@ -444,7 +483,7 @@
   </autoFilter>
   <tableColumns count="18">
     <tableColumn id="17" name="ID"/>
-    <tableColumn id="1" name="Funcionalidad"/>
+    <tableColumn id="1" name="Funcionalidad" dataDxfId="3"/>
     <tableColumn id="18" name="Rol"/>
     <tableColumn id="16" name="Sprint"/>
     <tableColumn id="2" name="2-sep-11"/>
@@ -470,7 +509,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B16" totalsRowShown="0">
   <autoFilter ref="A1:B16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="ID"/>
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
     <tableColumn id="2" name="Descripcion estado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -478,7 +517,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -552,7 +591,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -587,7 +625,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -763,14 +800,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="97.28515625" bestFit="1" customWidth="1"/>
@@ -785,7 +822,7 @@
     <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -841,7 +878,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -855,7 +892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -883,7 +920,7 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -911,7 +948,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -939,7 +976,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
@@ -967,7 +1004,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
@@ -995,7 +1032,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1023,7 +1060,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1051,7 +1088,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1068,7 +1105,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1096,7 +1133,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1124,7 +1161,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1152,7 +1189,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1180,7 +1217,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="45" hidden="1">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1208,7 +1245,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1225,7 +1262,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1242,7 +1279,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1270,7 +1307,7 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1298,7 +1335,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1326,7 +1363,7 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30" hidden="1">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1340,7 +1377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1368,7 +1405,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
-    <row r="23" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="45" hidden="1">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1382,7 +1419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1396,7 +1433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1424,7 +1461,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1452,7 +1489,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1480,7 +1517,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1508,7 +1545,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1522,7 +1559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="30" hidden="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1550,7 +1587,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" hidden="1">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1564,7 +1601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1592,7 +1629,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1620,7 +1657,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1648,7 +1685,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1676,12 +1713,12 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2">
@@ -1703,6 +1740,7 @@
       <c r="R36" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
@@ -1712,19 +1750,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="191.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1732,15 +1770,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1748,39 +1786,39 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60">
       <c r="A5" s="2">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="150">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="75">
       <c r="A7" s="2">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>11</v>
       </c>
@@ -1788,67 +1826,68 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="30">
       <c r="A9" s="2">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="2">
         <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="315">
       <c r="A15" s="2">
         <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
@@ -1858,40 +1897,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="20.25" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1"/>
+    <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>